<commit_message>
final commit for 12/16
</commit_message>
<xml_diff>
--- a/Data Dictionary.xlsx
+++ b/Data Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cumccolumbia-my.sharepoint.com/personal/qra2000_cumc_columbia_edu/Documents/Behavioral Health RC/AAAV4952 Loneliness/loneliness/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="380" documentId="8_{89E09587-57B3-4753-8A41-82410DD0F6D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E8C3BCE-E336-451D-94AF-C7AB08A55E5B}"/>
+  <xr:revisionPtr revIDLastSave="383" documentId="8_{89E09587-57B3-4753-8A41-82410DD0F6D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E709EE8E-1DE7-4614-A129-6E13F9959A05}"/>
   <bookViews>
-    <workbookView xWindow="-57705" yWindow="0" windowWidth="16290" windowHeight="15585" xr2:uid="{798B117E-ED49-4CC2-A2A3-613410427F1F}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{798B117E-ED49-4CC2-A2A3-613410427F1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -543,7 +543,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -553,6 +553,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -584,7 +590,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -601,6 +607,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -622,7 +629,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -959,15 +966,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E93C2329-9D1A-4EC0-8D2B-816A65EB75D3}">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="4"/>
     <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38" style="1" customWidth="1"/>
+    <col min="3" max="3" width="72.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="25.42578125" customWidth="1"/>
     <col min="5" max="5" width="22.140625" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
@@ -994,817 +1001,829 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="7">
         <v>19</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
     </row>
     <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="7"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="8"/>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="A5" s="7">
         <v>20</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="7"/>
+      <c r="F5" s="8"/>
     </row>
     <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+      <c r="A6" s="7">
         <v>22</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="7"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="A7" s="7">
         <v>23</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="7"/>
+      <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="A8" s="7">
         <v>24</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="7"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="8"/>
     </row>
     <row r="9" spans="1:7" ht="195" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+      <c r="A9" s="7">
         <v>39</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7" t="s">
+      <c r="E9" s="8"/>
+      <c r="F9" s="8" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="210" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+      <c r="A10" s="7">
         <v>51</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7" t="s">
+      <c r="E10" s="8"/>
+      <c r="F10" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+      <c r="A11" s="7">
         <v>55</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="8" t="s">
+      <c r="D11" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="9" t="s">
         <v>132</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G11" s="15"/>
+      <c r="G11" s="16"/>
     </row>
     <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
+      <c r="A12" s="7">
         <v>56</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="7"/>
+      <c r="D12" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="8"/>
       <c r="F12" t="s">
         <v>112</v>
       </c>
-      <c r="G12" s="15"/>
+      <c r="G12" s="16"/>
     </row>
     <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+      <c r="A13" s="7">
         <v>57</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" s="7"/>
+      <c r="D13" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="8"/>
       <c r="F13" t="s">
         <v>113</v>
       </c>
-      <c r="G13" s="15"/>
+      <c r="G13" s="16"/>
     </row>
     <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
+      <c r="A14" s="7">
         <v>58</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="7"/>
+      <c r="D14" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="8"/>
       <c r="F14" t="s">
         <v>114</v>
       </c>
-      <c r="G14" s="15"/>
+      <c r="G14" s="16"/>
     </row>
     <row r="15" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
+      <c r="A15" s="7">
         <v>59</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="8" t="s">
+      <c r="D15" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="9" t="s">
         <v>132</v>
       </c>
       <c r="F15" t="s">
         <v>115</v>
       </c>
-      <c r="G15" s="15"/>
+      <c r="G15" s="16"/>
     </row>
     <row r="16" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
+      <c r="A16" s="7">
         <v>60</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E16" s="8" t="s">
+      <c r="D16" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="9" t="s">
         <v>132</v>
       </c>
       <c r="F16" t="s">
         <v>116</v>
       </c>
-      <c r="G16" s="15"/>
+      <c r="G16" s="16"/>
     </row>
     <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
+      <c r="A17" s="7">
         <v>61</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E17" s="7"/>
+      <c r="D17" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="8"/>
       <c r="F17" t="s">
         <v>117</v>
       </c>
-      <c r="G17" s="15"/>
+      <c r="G17" s="16"/>
     </row>
     <row r="18" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
+      <c r="A18" s="7">
         <v>62</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" s="7"/>
+      <c r="D18" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="8"/>
       <c r="F18" t="s">
         <v>118</v>
       </c>
-      <c r="G18" s="15"/>
+      <c r="G18" s="16"/>
     </row>
     <row r="19" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
+      <c r="A19" s="7">
         <v>63</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="D19" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19" s="8" t="s">
+      <c r="D19" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="9" t="s">
         <v>132</v>
       </c>
       <c r="F19" t="s">
         <v>119</v>
       </c>
-      <c r="G19" s="15"/>
+      <c r="G19" s="16"/>
     </row>
     <row r="20" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
+      <c r="A20" s="7">
         <v>64</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20" s="8" t="s">
+      <c r="D20" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="9" t="s">
         <v>132</v>
       </c>
       <c r="F20" t="s">
         <v>120</v>
       </c>
+      <c r="G20" s="6"/>
     </row>
     <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
+      <c r="A21" s="7">
         <v>65</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D21" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E21" s="7"/>
+      <c r="D21" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="8"/>
       <c r="F21" t="s">
         <v>121</v>
       </c>
+      <c r="G21" s="6"/>
     </row>
     <row r="22" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
+      <c r="A22" s="7">
         <v>66</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="D22" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E22" s="7"/>
+      <c r="D22" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" s="8"/>
       <c r="F22" t="s">
         <v>122</v>
       </c>
+      <c r="G22" s="6"/>
     </row>
     <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="6">
+      <c r="A23" s="7">
         <v>67</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D23" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" s="7"/>
+      <c r="D23" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="8"/>
       <c r="F23" t="s">
         <v>123</v>
       </c>
+      <c r="G23" s="6"/>
     </row>
     <row r="24" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="6">
+      <c r="A24" s="7">
         <v>68</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" s="7"/>
+      <c r="D24" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="8"/>
       <c r="F24" t="s">
         <v>124</v>
       </c>
+      <c r="G24" s="6"/>
     </row>
     <row r="25" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A25" s="6">
+      <c r="A25" s="7">
         <v>69</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="D25" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E25" s="8" t="s">
+      <c r="D25" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25" s="9" t="s">
         <v>132</v>
       </c>
       <c r="F25" t="s">
         <v>125</v>
       </c>
+      <c r="G25" s="6"/>
     </row>
     <row r="26" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A26" s="6">
+      <c r="A26" s="7">
         <v>70</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="D26" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E26" s="8" t="s">
+      <c r="D26" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" s="9" t="s">
         <v>132</v>
       </c>
       <c r="F26" t="s">
         <v>126</v>
       </c>
+      <c r="G26" s="6"/>
     </row>
     <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" s="6">
+      <c r="A27" s="7">
         <v>71</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="D27" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E27" s="7"/>
+      <c r="D27" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" s="8"/>
       <c r="F27" t="s">
         <v>127</v>
       </c>
+      <c r="G27" s="6"/>
     </row>
     <row r="28" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="6">
+      <c r="A28" s="7">
         <v>72</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="D28" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E28" s="7"/>
+      <c r="D28" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" s="8"/>
       <c r="F28" t="s">
         <v>128</v>
       </c>
+      <c r="G28" s="6"/>
     </row>
     <row r="29" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A29" s="6">
+      <c r="A29" s="7">
         <v>73</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="D29" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E29" s="8" t="s">
+      <c r="D29" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="9" t="s">
         <v>132</v>
       </c>
       <c r="F29" t="s">
         <v>129</v>
       </c>
+      <c r="G29" s="6"/>
     </row>
     <row r="30" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A30" s="6">
+      <c r="A30" s="7">
         <v>74</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D30" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E30" s="8" t="s">
+      <c r="D30" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E30" s="9" t="s">
         <v>132</v>
       </c>
       <c r="F30" t="s">
         <v>130</v>
       </c>
+      <c r="G30" s="6"/>
     </row>
     <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="14" t="s">
+      <c r="C31" s="9"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="F31" s="11"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="6"/>
     </row>
     <row r="32" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A32" s="6">
+      <c r="A32" s="7">
         <v>76</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
     </row>
     <row r="33" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A33" s="6">
+      <c r="A33" s="7">
         <v>77</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
     </row>
     <row r="34" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A34" s="6">
+      <c r="A34" s="7">
         <v>78</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
     </row>
     <row r="35" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A35" s="6">
+      <c r="A35" s="7">
         <v>79</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
     </row>
     <row r="36" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A36" s="6">
+      <c r="A36" s="7">
         <v>80</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
     </row>
     <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="6">
+      <c r="A37" s="7">
         <v>81</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D37" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E37" s="8" t="s">
+      <c r="E37" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="F37" s="7"/>
+      <c r="F37" s="8"/>
     </row>
     <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="6">
+      <c r="A38" s="7">
         <v>84</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C38" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D38" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E38" s="8" t="s">
+      <c r="E38" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="F38" s="7"/>
+      <c r="F38" s="8"/>
     </row>
     <row r="39" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="A39" s="6">
+      <c r="A39" s="7">
         <v>85</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D39" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E39" s="8" t="s">
+      <c r="E39" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="F39" s="7"/>
+      <c r="F39" s="8"/>
     </row>
     <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="6">
+      <c r="A40" s="7">
         <v>88</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C40" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="D40" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E40" s="8" t="s">
+      <c r="E40" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="F40" s="7"/>
+      <c r="F40" s="8"/>
     </row>
     <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="6">
+      <c r="A41" s="7">
         <v>91</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="C41" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="D41" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E41" s="8" t="s">
+      <c r="E41" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="F41" s="7"/>
+      <c r="F41" s="8"/>
     </row>
     <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="6">
+      <c r="A42" s="7">
         <v>94</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="C42" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="D42" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E42" s="8" t="s">
+      <c r="E42" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="F42" s="7"/>
+      <c r="F42" s="8"/>
     </row>
     <row r="43" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="6">
+      <c r="A43" s="7">
         <v>97</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C43" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="D43" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E43" s="8" t="s">
+      <c r="E43" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="F43" s="7"/>
+      <c r="F43" s="8"/>
     </row>
     <row r="44" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="6">
+      <c r="A44" s="7">
         <v>100</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="C44" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="D44" s="8" t="s">
+      <c r="D44" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E44" s="8" t="s">
+      <c r="E44" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="F44" s="7"/>
+      <c r="F44" s="8"/>
     </row>
     <row r="45" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="6">
+      <c r="A45" s="7">
         <v>103</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="C45" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="D45" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E45" s="8" t="s">
+      <c r="E45" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="F45" s="7"/>
+      <c r="F45" s="8"/>
     </row>
     <row r="46" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A46" s="6">
+      <c r="A46" s="7">
         <v>106</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B46" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="C46" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="D46" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E46" s="8" t="s">
+      <c r="E46" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="F46" s="7"/>
+      <c r="F46" s="8"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F46" xr:uid="{E93C2329-9D1A-4EC0-8D2B-816A65EB75D3}"/>

</xml_diff>